<commit_message>
Calculate and plot cumulative fluxes
</commit_message>
<xml_diff>
--- a/data/DWP2013 headspace_cm.xlsx
+++ b/data/DWP2013 headspace_cm.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="13395" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="40" windowWidth="17840" windowHeight="15700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -363,16 +368,16 @@
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -380,7 +385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -388,7 +393,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -396,7 +401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -404,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -412,7 +417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -420,7 +425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -428,7 +433,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -436,7 +441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -444,7 +449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -452,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -460,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -468,7 +473,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -476,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -484,7 +489,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -492,7 +497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -500,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -508,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -516,7 +521,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -524,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -532,7 +537,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -540,7 +545,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -548,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -556,15 +561,15 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>3.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -572,7 +577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -580,7 +585,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -588,7 +593,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -596,7 +601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -604,7 +609,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -612,7 +617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -620,7 +625,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -628,7 +633,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -636,7 +641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -644,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -652,7 +657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -660,7 +665,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -668,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -676,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -684,7 +689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -692,7 +697,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -700,7 +705,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>39</v>
       </c>
@@ -708,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -716,7 +721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>41</v>
       </c>
@@ -724,7 +729,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>42</v>
       </c>
@@ -732,7 +737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>43</v>
       </c>
@@ -740,7 +745,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>44</v>
       </c>
@@ -748,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>45</v>
       </c>
@@ -756,7 +761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>46</v>
       </c>
@@ -764,7 +769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>47</v>
       </c>
@@ -772,7 +777,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>48</v>
       </c>
@@ -780,7 +785,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>49</v>
       </c>
@@ -788,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>50</v>
       </c>
@@ -796,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>51</v>
       </c>
@@ -804,7 +809,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>52</v>
       </c>
@@ -812,7 +817,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>53</v>
       </c>
@@ -825,6 +830,11 @@
     <sortCondition ref="A2:A56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -834,9 +844,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -846,8 +861,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>